<commit_message>
Ajustado el codigo para que el hisotgrama de jugadores de <= 50 partidas se genere
</commit_message>
<xml_diff>
--- a/Modelizacion/Cargas_Componentes_PCR.xlsx
+++ b/Modelizacion/Cargas_Componentes_PCR.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">0.377720651721</t>
+    <t xml:space="preserve">0.377720651720999</t>
   </si>
   <si>
     <t xml:space="preserve">0.316730776239899</t>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">0.0766733070063346</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0578427308366979</t>
+    <t xml:space="preserve">0.0578427308366978</t>
   </si>
   <si>
     <t xml:space="preserve">0.340430560194557</t>
@@ -68,136 +68,136 @@
     <t xml:space="preserve">-0.02134667196672</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00265662274728414</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0877076024317945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.208441949215791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.432389624401581</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0915039438736426</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00107453039952041</t>
+    <t xml:space="preserve">0.00265662274728267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0877076024317933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.208441949215786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.432389624401578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09150394387364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00107453039951997</t>
   </si>
   <si>
     <t xml:space="preserve">-0.218965170896313</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.386203059479824</t>
+    <t xml:space="preserve">-0.386203059479828</t>
   </si>
   <si>
     <t xml:space="preserve">0.132109962445391</t>
   </si>
   <si>
-    <t xml:space="preserve">0.247683389711162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.271475258524769</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0370891019858972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.284993297022984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0538230694695115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.15885055651925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.289320791457324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.457696588087047</t>
+    <t xml:space="preserve">0.247683389711166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.271475258524775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0370891019858964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.284993297022982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0538230694695133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.158850556519255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.289320791457323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.457696588087044</t>
   </si>
   <si>
     <t xml:space="preserve">0.121316446863025</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0897226426660739</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.409868717153016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.176597940172607</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.215874064429813</t>
+    <t xml:space="preserve">-0.089722642666075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.409868717153018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.176597940172612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.215874064429814</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0593611786712282</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00674634307495577</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.315593959719183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.053843054060376</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.32378380070034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.476646989840983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0556344164569549</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.182968482285423</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.165252298091277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.39007628667349</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.170469177274892</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.219670081966928</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0923732446531611</t>
+    <t xml:space="preserve">-0.00674634307495864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.315593959719178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0538430540603777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.323783800700337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.47664698984098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0556344164569553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.182968482285427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.165252298091276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.390076286673488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.170469177274896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.219670081966933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.092373244653161</t>
   </si>
   <si>
     <t xml:space="preserve">0.117999925233253</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.385133554212022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.431519554262847</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0351254093600801</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.416689288537133</t>
+    <t xml:space="preserve">-0.385133554212021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.431519554262846</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03512540936008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.416689288537132</t>
   </si>
   <si>
     <t xml:space="preserve">0.286402717500167</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0154914920555959</t>
+    <t xml:space="preserve">-0.0154914920555961</t>
   </si>
   <si>
     <t xml:space="preserve">-0.281149214128831</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.079742342316598</t>
+    <t xml:space="preserve">-0.0797423423165978</t>
   </si>
   <si>
     <t xml:space="preserve">-0.139014393975394</t>
@@ -206,244 +206,244 @@
     <t xml:space="preserve">-0.146777807472815</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.286173831780724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0128231193796064</t>
+    <t xml:space="preserve">-0.286173831780723</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0128231193796066</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0290174823476656</t>
   </si>
   <si>
-    <t xml:space="preserve">0.157294779258229</t>
+    <t xml:space="preserve">0.157294779258228</t>
   </si>
   <si>
     <t xml:space="preserve">0.389820415103508</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0417714547514223</t>
+    <t xml:space="preserve">0.0417714547514221</t>
   </si>
   <si>
     <t xml:space="preserve">0.120343828687012</t>
   </si>
   <si>
-    <t xml:space="preserve">0.182085754563482</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0224200008910678</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0655339998901092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.556193452192447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.000605457903119309</t>
+    <t xml:space="preserve">0.182085754563485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0224200008910655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0655339998901099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.556193452192439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.000605457903121331</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0620720785948144</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.778071830989809</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0584913285016593</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0246565547610748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00466602276587982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0580174767165309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0667591716960273</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0462795695395724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0360730087555453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.109100214518083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0238420826401808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0161955925659057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.391663919977093</t>
+    <t xml:space="preserve">-0.778071830989812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0584913285016594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0246565547610754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00466602276587914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0580174767165293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0667591716960279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0462795695395726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0360730087555446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.109100214518081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.023842082640181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.016195592565906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.391663919977092</t>
   </si>
   <si>
     <t xml:space="preserve">-0.229989992579541</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0611637104972273</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.715559513628097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.157937558132808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00203967100984726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.443901674004776</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0489179611256594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0687181897102577</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0751797708125613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.14054815693895</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0448672237688737</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0308449055808446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0880447251662091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.108960546837106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0293862540260997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.452018562251528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.111349020977927</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0276606231817122</t>
+    <t xml:space="preserve">-0.0611637104972265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.715559513628102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.157937558132809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00203967100984719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.44390167400477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0489179611256582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0687181897102574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0751797708125612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.140548156938951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0448672237688731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0308449055808443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0880447251662089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.108960546837107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0293862540260991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.452018562251525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.111349020977928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0276606231817119</t>
   </si>
   <si>
     <t xml:space="preserve">0.190197767067664</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00976862188449335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.240643653211882</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.304566888605851</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.10744399783159</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.68078950533898</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.201726678523681</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0828179942300098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0475266379323234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.106225322906742</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00430872206362096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.241170963917925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0203799695940779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0355157306922651</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.408429853017878</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0174414947299244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0529290691771403</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0863791864767089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0286743797747075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.476804825912701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0768667034092334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0926347456219135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.527937865500228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.340353671407114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.159742657762016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0819695789719711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.178628466541036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.26303058152312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.216392494387053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0631444080081271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0740796497310735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.163262119083233</t>
+    <t xml:space="preserve">-0.0097686218844926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.240643653211875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.304566888605852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.107443997831591</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.680789505338984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.201726678523683</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0828179942300095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0475266379323241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.10622532290674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0043087220636233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.241170963917923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0203799695940784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.035515730692266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.40842985301788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0174414947299275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0529290691771418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0863791864767084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0286743797747071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.476804825912709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0768667034092339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0926347456219131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52793786550022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.340353671407111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.159742657762015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0819695789719704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.178628466541038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.263030581523121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.216392494387055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0631444080081276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0740796497310736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.163262119083234</t>
   </si>
   <si>
     <t xml:space="preserve">-0.466250496977956</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0551529627987263</t>
+    <t xml:space="preserve">0.0551529627987247</t>
   </si>
   <si>
     <t xml:space="preserve">0.303861522931845</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00563068486851631</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.642466141836255</t>
+    <t xml:space="preserve">-0.0056306848685168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.642466141836252</t>
   </si>
   <si>
     <t xml:space="preserve">0.265629363535784</t>
@@ -452,73 +452,73 @@
     <t xml:space="preserve">-0.182373387473474</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.181584625794662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.180036396117848</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.232122264009453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0172107564889631</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0798291440282893</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0509304460325253</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.099753594141873</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000780006120585475</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0690176021440521</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.166790992418304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.119209021679964</t>
+    <t xml:space="preserve">-0.181584625794668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.180036396117852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.232122264009454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0172107564889633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0798291440282881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0509304460325233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.099753594141874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000780006120587692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0690176021440517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.166790992418305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.119209021679963</t>
   </si>
   <si>
     <t xml:space="preserve">-0.690464072439992</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0318082163963433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00856160288526105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0150997995383505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00942527531826108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0755518559040896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0248566739188845</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.065220881336605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0252596583153126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0267453774435463</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0227188095493833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0400702557265401</t>
+    <t xml:space="preserve">0.0318082163963427</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00856160288526082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0150997995383497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00942527531826033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0755518559040903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0248566739188858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0652208813366058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0252596583153115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0267453774435466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0227188095493829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0400702557265399</t>
   </si>
   <si>
     <t xml:space="preserve">-0.106885874089335</t>
@@ -527,7 +527,7 @@
     <t xml:space="preserve">0.670510685941486</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.070281727084939</t>
+    <t xml:space="preserve">-0.0702817270849391</t>
   </si>
   <si>
     <t xml:space="preserve">0.0618806815926293</t>
@@ -536,13 +536,13 @@
     <t xml:space="preserve">-0.395907123408838</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0787124144187174</t>
+    <t xml:space="preserve">-0.0787124144187178</t>
   </si>
   <si>
     <t xml:space="preserve">0.0735026592186972</t>
   </si>
   <si>
-    <t xml:space="preserve">0.000793861399298584</t>
+    <t xml:space="preserve">0.000793861399298554</t>
   </si>
   <si>
     <t xml:space="preserve">0.124250169190045</t>
@@ -554,109 +554,109 @@
     <t xml:space="preserve">-0.166634357502406</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0617331740982197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.377489681172955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0048458576918168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.686041304551935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0682170840917607</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0187688943376601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0629003835152528</t>
+    <t xml:space="preserve">-0.0617331740982195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.377489681172954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00484585769181658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.686041304551934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0682170840917594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0187688943376604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0629003835152536</t>
   </si>
   <si>
     <t xml:space="preserve">-0.154904932809209</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0113135790299048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0591306781530014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0000326167253205598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0506710898394325</t>
+    <t xml:space="preserve">0.0113135790299045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0591306781530019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0000326167253207723</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0506710898394326</t>
   </si>
   <si>
     <t xml:space="preserve">0.146425507256368</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00319460498940746</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0730943283859082</t>
+    <t xml:space="preserve">-0.00319460498940744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0730943283859087</t>
   </si>
   <si>
     <t xml:space="preserve">0.256482367697769</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0580120949709909</t>
+    <t xml:space="preserve">-0.0580120949709911</t>
   </si>
   <si>
     <t xml:space="preserve">0.100223997569025</t>
   </si>
   <si>
-    <t xml:space="preserve">0.435945368211031</t>
+    <t xml:space="preserve">0.435945368211032</t>
   </si>
   <si>
     <t xml:space="preserve">-0.385936110180949</t>
   </si>
   <si>
-    <t xml:space="preserve">0.326739649928961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.383403156089748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.43124383622222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.324741462012026</t>
+    <t xml:space="preserve">0.326739649928962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.383403156089747</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.431243836222221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.324741462012025</t>
   </si>
   <si>
     <t xml:space="preserve">0.0603410684395936</t>
   </si>
   <si>
-    <t xml:space="preserve">0.126927974469249</t>
+    <t xml:space="preserve">0.126927974469248</t>
   </si>
   <si>
     <t xml:space="preserve">-0.195744797014492</t>
   </si>
   <si>
-    <t xml:space="preserve">0.171167945338411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0418506471933789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0428933010529582</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00355033883888845</t>
+    <t xml:space="preserve">0.17116794533841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0418506471933787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0428933010529586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00355033883888859</t>
   </si>
   <si>
     <t xml:space="preserve">-0.220803802525662</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0247960576174992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00913143983568131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0505876912944307</t>
+    <t xml:space="preserve">-0.0247960576174994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00913143983568107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0505876912944305</t>
   </si>
   <si>
     <t xml:space="preserve">-0.332551690434044</t>
@@ -665,7 +665,7 @@
     <t xml:space="preserve">0.226570741441283</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0106132773457059</t>
+    <t xml:space="preserve">-0.0106132773457047</t>
   </si>
   <si>
     <t xml:space="preserve">-0.588096414720692</t>
@@ -677,160 +677,160 @@
     <t xml:space="preserve">0.50601699929916</t>
   </si>
   <si>
-    <t xml:space="preserve">0.105240246865255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.134541995464661</t>
+    <t xml:space="preserve">0.105240246865256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.13454199546466</t>
   </si>
   <si>
     <t xml:space="preserve">0.476494223615876</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0658826790489282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00610155825561707</t>
+    <t xml:space="preserve">0.0658826790489281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00610155825561696</t>
   </si>
   <si>
     <t xml:space="preserve">0.464937999801023</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0102161435142209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00862780590849932</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0248783540162142</t>
+    <t xml:space="preserve">0.010216143514221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0086278059084985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0248783540162128</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0192208451389713</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0400473054939179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0569702230702231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.12585728838342</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.227735172290981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.445777785956285</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.121827930062296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.438348814448901</t>
+    <t xml:space="preserve">-0.0400473054939181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0569702230702237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.125857288383423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.22773517229098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.445777785956284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.121827930062299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.4383488144489</t>
   </si>
   <si>
     <t xml:space="preserve">-0.234258624987557</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0993657944619896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.052829781106483</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0446135473790701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0475987389031175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.172568207387078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0096812565246671</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.130655333488761</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.449273487010498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00442794275027685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0318863846015127</t>
+    <t xml:space="preserve">0.09936579446199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0528297811064809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0446135473790704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0475987389031176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17256820738708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00968125652466711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.13065533348876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.449273487010499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00442794275027683</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0318863846015124</t>
   </si>
   <si>
     <t xml:space="preserve">0.111193070781612</t>
   </si>
   <si>
-    <t xml:space="preserve">0.548716370687277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.207550963047563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0829671018654749</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.606111304848873</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0474013368804018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0148257825545064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0900708848782516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.310081288896272</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0826177597808817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.188946293436606</t>
+    <t xml:space="preserve">0.548716370687276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.207550963047564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0829671018654767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.606111304848872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0474013368803999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0148257825545076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0900708848782517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.310081288896273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0826177597808815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.188946293436605</t>
   </si>
   <si>
     <t xml:space="preserve">-0.596027655217278</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00209218677391483</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0269734495079006</t>
+    <t xml:space="preserve">-0.00209218677391488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.026973449507901</t>
   </si>
   <si>
     <t xml:space="preserve">0.343171062463952</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0156794377834471</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0376754431585803</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0246309027477707</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.41340223587165</t>
+    <t xml:space="preserve">0.0156794377834469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0376754431585802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0246309027477706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.413402235871649</t>
   </si>
   <si>
     <t xml:space="preserve">0.168670589076611</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.298845940630852</t>
+    <t xml:space="preserve">-0.298845940630853</t>
   </si>
   <si>
     <t xml:space="preserve">-0.110252124656463</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.269453454738512</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0614036882093608</t>
+    <t xml:space="preserve">-0.269453454738513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0614036882093605</t>
   </si>
   <si>
     <t xml:space="preserve">-0.872991414517956</t>
@@ -842,37 +842,37 @@
     <t xml:space="preserve">0.0655473532529584</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0838575449918505</t>
+    <t xml:space="preserve">0.0838575449918504</t>
   </si>
   <si>
     <t xml:space="preserve">0.230225559034324</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00175870982129913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0321204420432243</t>
+    <t xml:space="preserve">-0.00175870982129934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0321204420432242</t>
   </si>
   <si>
     <t xml:space="preserve">0.144299209575821</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.000195844917782795</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0031110065645539</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0202187647933168</t>
+    <t xml:space="preserve">-0.000195844917782857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00311100656455408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0202187647933166</t>
   </si>
   <si>
     <t xml:space="preserve">0.254978231146432</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00707821164339111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00172106859702142</t>
+    <t xml:space="preserve">0.00707821164339122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00172106859702106</t>
   </si>
   <si>
     <t xml:space="preserve">0.0305923651932767</t>

</xml_diff>

<commit_message>
Nuevos ajustes al PCR
</commit_message>
<xml_diff>
--- a/Modelizacion/Cargas_Componentes_PCR.xlsx
+++ b/Modelizacion/Cargas_Componentes_PCR.xlsx
@@ -12,876 +12,1092 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="362">
   <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">0.377720651720999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.316730776239899</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0766733070063346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0578427308366978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.340430560194557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0147275230221164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.241567544545824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.201592790723588</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0849368122859007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.159360533827578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.146595078057632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.358143685192719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.263309838168161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.347357894329287</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.279293999613654</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.286115876524038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.02134667196672</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00265662274728267</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0877076024317933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.208441949215786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.432389624401578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09150394387364</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00107453039951997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.218965170896313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.386203059479828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.132109962445391</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.247683389711166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.271475258524775</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0370891019858964</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.284993297022982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0538230694695133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.158850556519255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.289320791457323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.457696588087044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.121316446863025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.089722642666075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.409868717153018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.176597940172612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.215874064429814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0593611786712282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00674634307495864</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.315593959719178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0538430540603777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.323783800700337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.47664698984098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0556344164569553</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.182968482285427</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.165252298091276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.390076286673488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.170469177274896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.219670081966933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.092373244653161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.117999925233253</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.385133554212021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.431519554262846</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03512540936008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.416689288537132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.286402717500167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0154914920555961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.281149214128831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0797423423165978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.139014393975394</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.146777807472815</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.286173831780723</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0128231193796066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0290174823476656</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.157294779258228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.389820415103508</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0417714547514221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.120343828687012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.182085754563485</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0224200008910655</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0655339998901099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.556193452192439</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.000605457903121331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0620720785948144</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.778071830989812</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0584913285016594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0246565547610754</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00466602276587914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0580174767165293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0667591716960279</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0462795695395726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0360730087555446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.109100214518081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.023842082640181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.016195592565906</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.391663919977092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.229989992579541</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0611637104972265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.715559513628102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.157937558132809</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00203967100984719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.44390167400477</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0489179611256582</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0687181897102574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0751797708125612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.140548156938951</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0448672237688731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0308449055808443</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0880447251662089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.108960546837107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0293862540260991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.452018562251525</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.111349020977928</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0276606231817119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.190197767067664</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0097686218844926</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.240643653211875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.304566888605852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.107443997831591</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.680789505338984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.201726678523683</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0828179942300095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0475266379323241</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.10622532290674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0043087220636233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.241170963917923</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0203799695940784</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.035515730692266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.40842985301788</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0174414947299275</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0529290691771418</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0863791864767084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0286743797747071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.476804825912709</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0768667034092339</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0926347456219131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.52793786550022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.340353671407111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.159742657762015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0819695789719704</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.178628466541038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.263030581523121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.216392494387055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0631444080081276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0740796497310736</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.163262119083234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.466250496977956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0551529627987247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.303861522931845</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0056306848685168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.642466141836252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.265629363535784</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.182373387473474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.181584625794668</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.180036396117852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.232122264009454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0172107564889633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0798291440282881</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0509304460325233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.099753594141874</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000780006120587692</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0690176021440517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.166790992418305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.119209021679963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.690464072439992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0318082163963427</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00856160288526082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0150997995383497</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00942527531826033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0755518559040903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0248566739188858</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0652208813366058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0252596583153115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0267453774435466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0227188095493829</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0400702557265399</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.106885874089335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.670510685941486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0702817270849391</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0618806815926293</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.395907123408838</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0787124144187178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0735026592186972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000793861399298554</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.124250169190045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.360196258012139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.166634357502406</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0617331740982195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.377489681172954</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00484585769181658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.686041304551934</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0682170840917594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0187688943376604</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0629003835152536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.154904932809209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0113135790299045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0591306781530019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0000326167253207723</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0506710898394326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.146425507256368</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00319460498940744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0730943283859087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.256482367697769</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0580120949709911</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.100223997569025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.435945368211032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.385936110180949</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.326739649928962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.383403156089747</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.431243836222221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.324741462012025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0603410684395936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.126927974469248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.195744797014492</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.17116794533841</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0418506471933787</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0428933010529586</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00355033883888859</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.220803802525662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0247960576174994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00913143983568107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0505876912944305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.332551690434044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.226570741441283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0106132773457047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.588096414720692</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.292635514757961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.50601699929916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.105240246865256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.13454199546466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.476494223615876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0658826790489281</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00610155825561696</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.464937999801023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.010216143514221</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0086278059084985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0248783540162128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0192208451389713</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0400473054939181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0569702230702237</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.125857288383423</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.22773517229098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.445777785956284</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.121827930062299</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.4383488144489</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.234258624987557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09936579446199</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0528297811064809</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0446135473790704</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0475987389031176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.17256820738708</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00968125652466711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.13065533348876</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.449273487010499</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00442794275027683</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0318863846015124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.111193070781612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.548716370687276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.207550963047564</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0829671018654767</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.606111304848872</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0474013368803999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0148257825545076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0900708848782517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.310081288896273</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0826177597808815</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.188946293436605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.596027655217278</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00209218677391488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.026973449507901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.343171062463952</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0156794377834469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0376754431585802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0246309027477706</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.413402235871649</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.168670589076611</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.298845940630853</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.110252124656463</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.269453454738513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0614036882093605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.872991414517956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2408954636203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0655473532529584</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0838575449918504</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.230225559034324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00175870982129934</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0321204420432242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.144299209575821</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.000195844917782857</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00311100656455408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0202187647933166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.254978231146432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00707821164339122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00172106859702106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0305923651932767</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.112888144005932</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.120419409119099</t>
+    <t xml:space="preserve">0.288674283245463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0318967039512507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0723093725973853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.272352274729438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00653417155006892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.228833149196094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.227584913920532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.072520215179904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.135187563983542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.137537209880377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.350738336783499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.202718114133101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.306362405912357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.258633338825256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.306241743394502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.161054836225144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.306769524542429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.27007690361451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.279211258109888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.127199436417685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.183177692336209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.428542928955178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.277731543262323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0262470112997947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0403734521138124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.113347706640329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0984099375672809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.180905804022954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.152387761508448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.116118006229621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.30349907771061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.178852760470267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.183228286382668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0431683833387373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.42450327445897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.238271374351827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.314719929192407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.315654696582483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0201851081415725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.250751722735524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0430109500712863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.207788347324384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0271856185713554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.160318546235123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.464459873999621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0211973231632182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.37926957649782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.53651997192287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00656646374215543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0510269449161907</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.223890116152415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.378777494378354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0255185596745931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0629959321745625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0375815454050994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0838171570578188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0898570758709144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.23251474327195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.526005869275801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.133201395957174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0394704506949973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.249023706465714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.37892999823513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0535307767166645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.283300239468071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0386063479161126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0505776867833565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0525443671205819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.386610629377029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.031916135045871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0810194830459721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.351832349210134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0866675388434688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.135865303821112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.173541381689862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.132270848447449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.129699465047593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11898515567183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0382185958990496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0579609351230582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.788633934031955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0224295391139462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0400263883740733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.561265377880051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0553333190949413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0329720255459619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0147201350817193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0562927461068497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0634576154566242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0557122045069946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0668899329970314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.032657130222181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0484665846931809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0194906295641944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0468838709265472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0179733113591751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.383296763658645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.117051312763791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0609208348094285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.558863152817506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.121407125294226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0263889817933262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.691115147542041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0544086642730107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0466004981559808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0425479126977789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.089950910275516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.060794025934634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0295361733794307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0772365011321741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0177304694969324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0141996430595281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0608582174811713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0125321726310835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.470007674763944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.149188963751005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.050494050336399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.204582583121948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0227273068998411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.221715309056876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.295368114694266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.135229029016298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.654063402710182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.202256694110346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.070216003677966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0592007574296007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.115662915022085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0163581514082419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.250708397789273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.019386802107489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0401701440428174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0149244222361573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.037070007787841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.419182672008471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0316405679670218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00694405210718372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.105623746197742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0335629401534712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.411348309286468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0785904477495109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.115743347643935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.559646642847283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.350869885209471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.159699230485412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.074612748736738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.182833019184808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247785593525533</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.220659183797969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0908610709324187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0516631657067299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0182641099764573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00372180854863112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.107555619664354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.418409217795567</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.346766504587756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.270571709328701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.016481179269691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.632098358370281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.175896568028657</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21674370368956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.182175897547229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11875869328456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.14502295537934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0189878326929793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0882026007486364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.104118822682027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0198819516732791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0276657336053235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.186367535654238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.070122843003225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.118562187673007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0984128375778727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.249748659138799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.651873306712827</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.135237102377568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00199888094333433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.213065332062043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.159170518349195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0437568325111204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00157901793540766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0360399324989038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.136746560298692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0158178175133112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0665231994012503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0324218897177772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.111079230803736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.474633849731984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.120684126851055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.211760505411164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.298849671504229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0663735679776274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.387464547097349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0638377794111176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0533749614132474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00178130314341117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.13667962596399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.402910910416706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.162664686477885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0665137888938199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.410829600516635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0236464490547476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.656411129579986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.108321984472389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0248743421535775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0684985243475422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0418447262001878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0336605608977063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0674152790072237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0441258738549835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0283950685560023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.116429729343358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0109771951216202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0707507145283178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00768429055683049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00781779871866108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.117848828538963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0250249145379952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.067362654127718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.123128587059695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.228265259086957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.174396898432001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.523967643792029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.187828348083848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48307346775372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.295301867250331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.458434960330218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0412122015679241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.146333275086964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.155426503625787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.145124313248951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0902608544267015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0864383682874608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0041610003633494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.179844098188617</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.202840355234028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0526225950928575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0954371249083252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.530586784665413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.378721114524699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.271401233021441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.132265671504604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.471547376668239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.156227506574572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.219011638132527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.205166137867467</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0277382332301585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00909105678064927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0222964816105981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.048678684920331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.290410122568354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.179704085087489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00509039341953729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.163178512971034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.198262037085476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00491842190486531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000731309249960996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0329744612013005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.160249236587388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.149308601524814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.344110088291943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.220403638680767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.245257253086963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.392434381092845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.412709691796925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.462008458850862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0230060251622762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.51147292231191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0832266634578485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0752816554266599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.486255622515938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00756706921689213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0345633827476928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0507603900132044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0214134738907788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0434710467042601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0669787452046161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.110608018109106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.264502322781098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.437499797647647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0699560996757531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.418302850041388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0404059464523267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0570369274761525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0984496033339909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.103164898693532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0698140914524312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0583761796600293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0355116724479262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.185932499213256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0076868268682995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.107114224104493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.390099666605517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00384670885783176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0305854991483807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.112554463430332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.581458877831682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170503932249089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.114974881097731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.588469879064148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.15169366629802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0223622870674415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.147578230248495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0392686629911759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0710121693113409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.029839195471503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0195353861806118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.317426995320424</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0708195379107083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00410891219953281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0790083777227831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.191289963235942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0178080606452021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0241912268063363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0174730019160098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0228690293729319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.109715054651705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247358949578326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.050165211069953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.208978135613688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0561038528699371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.532702659866491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.663992390535628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0339569657661886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.330662744555899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0763858986304451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11048863269772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.568497364664159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00398377208043602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0392141968089539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.338642707363421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0210348455172962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0407705870531164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0237683547185796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.408263864900699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.158443908946349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2540424607744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.105977135871593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.270245085446127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.168473390756013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0537476143409355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.179708641298495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.162406689795236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0665150644556144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0207529958212271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.109578914595145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0744068446517149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00847668665058336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.000783306696191217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0455418912541574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.000878509257945998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0173887767821311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0139581894397936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.221806585012749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0190552720971743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0611856151811291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0139621458682704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0888470334794383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.470887229281481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.194177812590604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.177731042380354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.789008763143683</t>
   </si>
 </sst>
 </file>
@@ -2663,6 +2879,366 @@
         <v>289</v>
       </c>
     </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s">
+        <v>361</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Eliminacion de chunks viejos y redundantes de codigo
</commit_message>
<xml_diff>
--- a/Modelizacion/Cargas_Componentes_PCR.xlsx
+++ b/Modelizacion/Cargas_Componentes_PCR.xlsx
@@ -20,16 +20,16 @@
     <t xml:space="preserve">0.288674283245463</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0318967039512505</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0723093725973854</t>
+    <t xml:space="preserve">0.0318967039512507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0723093725973853</t>
   </si>
   <si>
     <t xml:space="preserve">0.272352274729438</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00653417155006891</t>
+    <t xml:space="preserve">0.00653417155006892</t>
   </si>
   <si>
     <t xml:space="preserve">0.228833149196094</t>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">-0.0262470112997947</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0403734521138125</t>
+    <t xml:space="preserve">-0.0403734521138124</t>
   </si>
   <si>
     <t xml:space="preserve">0.113347706640329</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">-0.183228286382668</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0431683833387371</t>
+    <t xml:space="preserve">0.0431683833387373</t>
   </si>
   <si>
     <t xml:space="preserve">-0.42450327445897</t>
@@ -131,19 +131,19 @@
     <t xml:space="preserve">-0.315654696582483</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0201851081415726</t>
+    <t xml:space="preserve">0.0201851081415725</t>
   </si>
   <si>
     <t xml:space="preserve">0.250751722735524</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0430109500712859</t>
+    <t xml:space="preserve">0.0430109500712863</t>
   </si>
   <si>
     <t xml:space="preserve">0.207788347324384</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0271856185713557</t>
+    <t xml:space="preserve">-0.0271856185713554</t>
   </si>
   <si>
     <t xml:space="preserve">0.160318546235123</t>
@@ -161,43 +161,43 @@
     <t xml:space="preserve">-0.53651997192287</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00656646374215568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0510269449161909</t>
+    <t xml:space="preserve">-0.00656646374215543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0510269449161907</t>
   </si>
   <si>
     <t xml:space="preserve">0.223890116152415</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.378777494378355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0255185596745929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0629959321745623</t>
+    <t xml:space="preserve">-0.378777494378354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0255185596745931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0629959321745625</t>
   </si>
   <si>
     <t xml:space="preserve">0.0375815454050994</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0838171570578185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0898570758709142</t>
+    <t xml:space="preserve">0.0838171570578188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0898570758709144</t>
   </si>
   <si>
     <t xml:space="preserve">-0.23251474327195</t>
   </si>
   <si>
-    <t xml:space="preserve">0.526005869275802</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.133201395957175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0394704506949974</t>
+    <t xml:space="preserve">0.526005869275801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.133201395957174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0394704506949973</t>
   </si>
   <si>
     <t xml:space="preserve">-0.249023706465714</t>
@@ -206,7 +206,7 @@
     <t xml:space="preserve">-0.37892999823513</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0535307767166646</t>
+    <t xml:space="preserve">-0.0535307767166645</t>
   </si>
   <si>
     <t xml:space="preserve">0.283300239468071</t>
@@ -215,25 +215,25 @@
     <t xml:space="preserve">0.0386063479161126</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0505776867833564</t>
+    <t xml:space="preserve">0.0505776867833565</t>
   </si>
   <si>
     <t xml:space="preserve">0.0525443671205819</t>
   </si>
   <si>
-    <t xml:space="preserve">0.38661062937703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0319161350458707</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0810194830459723</t>
+    <t xml:space="preserve">0.386610629377029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.031916135045871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0810194830459721</t>
   </si>
   <si>
     <t xml:space="preserve">-0.351832349210134</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0866675388434687</t>
+    <t xml:space="preserve">-0.0866675388434688</t>
   </si>
   <si>
     <t xml:space="preserve">-0.135865303821112</t>
@@ -245,202 +245,202 @@
     <t xml:space="preserve">-0.132270848447449</t>
   </si>
   <si>
-    <t xml:space="preserve">0.129699465047595</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.118985155671831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0382185958990508</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0579609351230588</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.788633934031954</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.022429539113945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0400263883740738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.561265377880054</t>
+    <t xml:space="preserve">0.129699465047593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11898515567183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0382185958990496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0579609351230582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.788633934031955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0224295391139462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0400263883740733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.561265377880051</t>
   </si>
   <si>
     <t xml:space="preserve">0.0553333190949413</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0329720255459617</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0147201350817189</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0562927461068492</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.063457615456625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0557122045069942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0668899329970318</t>
+    <t xml:space="preserve">0.0329720255459619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0147201350817193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0562927461068497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0634576154566242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0557122045069946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0668899329970314</t>
   </si>
   <si>
     <t xml:space="preserve">0.032657130222181</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0484665846931812</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0194906295641941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0468838709265474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0179733113591748</t>
+    <t xml:space="preserve">0.0484665846931809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0194906295641944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0468838709265472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0179733113591751</t>
   </si>
   <si>
     <t xml:space="preserve">0.383296763658645</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.11705131276379</t>
+    <t xml:space="preserve">-0.117051312763791</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0609208348094285</t>
   </si>
   <si>
-    <t xml:space="preserve">0.55886315281751</t>
+    <t xml:space="preserve">0.558863152817506</t>
   </si>
   <si>
     <t xml:space="preserve">-0.121407125294226</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0263889817933263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.69111514754204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0544086642730094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0466004981559814</t>
+    <t xml:space="preserve">-0.0263889817933262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.691115147542041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0544086642730107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0466004981559808</t>
   </si>
   <si>
     <t xml:space="preserve">0.0425479126977789</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0899509102755157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0607940259346337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0295361733794308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0772365011321739</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0177304694969318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0141996430595287</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0608582174811712</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0125321726310839</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.470007674763945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.149188963751004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0504940503363989</t>
+    <t xml:space="preserve">0.089950910275516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.060794025934634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0295361733794307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0772365011321741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0177304694969324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0141996430595281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0608582174811713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0125321726310835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.470007674763944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.149188963751005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.050494050336399</t>
   </si>
   <si>
     <t xml:space="preserve">-0.204582583121948</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0227273068998418</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.221715309056877</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.295368114694267</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.135229029016299</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.654063402710183</t>
+    <t xml:space="preserve">0.0227273068998411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.221715309056876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.295368114694266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.135229029016298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.654063402710182</t>
   </si>
   <si>
     <t xml:space="preserve">0.202256694110346</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0702160036779664</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0592007574296004</t>
+    <t xml:space="preserve">-0.070216003677966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0592007574296007</t>
   </si>
   <si>
     <t xml:space="preserve">0.115662915022085</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0163581514082417</t>
+    <t xml:space="preserve">0.0163581514082419</t>
   </si>
   <si>
     <t xml:space="preserve">0.250708397789273</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0193868021074892</t>
+    <t xml:space="preserve">-0.019386802107489</t>
   </si>
   <si>
     <t xml:space="preserve">0.0401701440428174</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0149244222361574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0370700077878408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.419182672008472</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0316405679670227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00694405210718259</t>
+    <t xml:space="preserve">0.0149244222361573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.037070007787841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.419182672008471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0316405679670218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00694405210718372</t>
   </si>
   <si>
     <t xml:space="preserve">0.105623746197742</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0335629401534727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.411348309286466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0785904477495115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.115743347643936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.559646642847282</t>
+    <t xml:space="preserve">-0.0335629401534712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.411348309286468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0785904477495109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.115743347643935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.559646642847283</t>
   </si>
   <si>
     <t xml:space="preserve">0.350869885209471</t>
@@ -452,10 +452,10 @@
     <t xml:space="preserve">0.074612748736738</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.182833019184807</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.247785593525532</t>
+    <t xml:space="preserve">-0.182833019184808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247785593525533</t>
   </si>
   <si>
     <t xml:space="preserve">-0.220659183797969</t>
@@ -464,67 +464,67 @@
     <t xml:space="preserve">0.0908610709324187</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0516631657067302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0182641099764569</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00372180854863086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.107555619664353</t>
+    <t xml:space="preserve">-0.0516631657067299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0182641099764573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00372180854863112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.107555619664354</t>
   </si>
   <si>
     <t xml:space="preserve">0.418409217795567</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.346766504587755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2705717093287</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0164811792696919</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.632098358370282</t>
+    <t xml:space="preserve">-0.346766504587756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.270571709328701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.016481179269691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.632098358370281</t>
   </si>
   <si>
     <t xml:space="preserve">-0.175896568028657</t>
   </si>
   <si>
-    <t xml:space="preserve">0.216743703689559</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.182175897547227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.118758693284559</t>
+    <t xml:space="preserve">0.21674370368956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.182175897547229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.11875869328456</t>
   </si>
   <si>
     <t xml:space="preserve">-0.14502295537934</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0189878326929787</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0882026007486369</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.104118822682028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0198819516732787</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0276657336053233</t>
+    <t xml:space="preserve">-0.0189878326929793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0882026007486364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.104118822682027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0198819516732791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0276657336053235</t>
   </si>
   <si>
     <t xml:space="preserve">0.186367535654238</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0701228430032247</t>
+    <t xml:space="preserve">-0.070122843003225</t>
   </si>
   <si>
     <t xml:space="preserve">0.118562187673007</t>
@@ -533,7 +533,7 @@
     <t xml:space="preserve">0.0984128375778727</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.249748659138798</t>
+    <t xml:space="preserve">-0.249748659138799</t>
   </si>
   <si>
     <t xml:space="preserve">-0.651873306712827</t>
@@ -542,28 +542,28 @@
     <t xml:space="preserve">0.135237102377568</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00199888094333373</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.213065332062042</t>
+    <t xml:space="preserve">-0.00199888094333433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.213065332062043</t>
   </si>
   <si>
     <t xml:space="preserve">0.159170518349195</t>
   </si>
   <si>
-    <t xml:space="preserve">0.04375683251112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00157901793540709</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.036039932498904</t>
+    <t xml:space="preserve">0.0437568325111204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00157901793540766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0360399324989038</t>
   </si>
   <si>
     <t xml:space="preserve">0.136746560298692</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0158178175133105</t>
+    <t xml:space="preserve">-0.0158178175133112</t>
   </si>
   <si>
     <t xml:space="preserve">0.0665231994012503</t>
@@ -587,22 +587,22 @@
     <t xml:space="preserve">0.298849671504229</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0663735679776265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.387464547097347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.063837779411117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0533749614132472</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00178130314341074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.136679625963989</t>
+    <t xml:space="preserve">0.0663735679776274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.387464547097349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0638377794111176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0533749614132474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00178130314341117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.13667962596399</t>
   </si>
   <si>
     <t xml:space="preserve">-0.402910910416706</t>
@@ -614,127 +614,127 @@
     <t xml:space="preserve">-0.0665137888938199</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.410829600516636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.023646449054747</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.656411129579985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.108321984472391</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0248743421535766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0684985243475398</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0418447262001862</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0336605608977088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0674152790072236</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.044125873854983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0283950685560024</t>
+    <t xml:space="preserve">-0.410829600516635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0236464490547476</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.656411129579986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.108321984472389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0248743421535775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0684985243475422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0418447262001878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0336605608977063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0674152790072237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0441258738549835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0283950685560023</t>
   </si>
   <si>
     <t xml:space="preserve">0.116429729343358</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0109771951216195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0707507145283171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00768429055683044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00781779871866095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.117848828538964</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0250249145379945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0673626541277184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.123128587059697</t>
+    <t xml:space="preserve">-0.0109771951216202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0707507145283178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00768429055683049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00781779871866108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.117848828538963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0250249145379952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.067362654127718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.123128587059695</t>
   </si>
   <si>
     <t xml:space="preserve">-0.228265259086957</t>
   </si>
   <si>
-    <t xml:space="preserve">0.174396898431998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.523967643792027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.187828348083849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.483073467753719</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.295301867250332</t>
+    <t xml:space="preserve">0.174396898432001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.523967643792029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.187828348083848</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48307346775372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.295301867250331</t>
   </si>
   <si>
     <t xml:space="preserve">-0.458434960330218</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0412122015679232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.146333275086965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.155426503625788</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.145124313248952</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0902608544267012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.086438368287461</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00416100036334958</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.179844098188618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.202840355234026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0526225950928586</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.095437124908325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.530586784665411</t>
+    <t xml:space="preserve">0.0412122015679241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.146333275086964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.155426503625787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.145124313248951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0902608544267015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0864383682874608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0041610003633494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.179844098188617</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.202840355234028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0526225950928575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0954371249083252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.530586784665413</t>
   </si>
   <si>
     <t xml:space="preserve">-0.378721114524699</t>
   </si>
   <si>
-    <t xml:space="preserve">0.271401233021443</t>
+    <t xml:space="preserve">0.271401233021441</t>
   </si>
   <si>
     <t xml:space="preserve">0.132265671504604</t>
@@ -743,7 +743,7 @@
     <t xml:space="preserve">-0.471547376668239</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.156227506574574</t>
+    <t xml:space="preserve">-0.156227506574572</t>
   </si>
   <si>
     <t xml:space="preserve">-0.219011638132527</t>
@@ -752,25 +752,25 @@
     <t xml:space="preserve">0.205166137867467</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0277382332301578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00909105678064961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0222964816105982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0486786849203308</t>
+    <t xml:space="preserve">0.0277382332301585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00909105678064927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0222964816105981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.048678684920331</t>
   </si>
   <si>
     <t xml:space="preserve">0.290410122568354</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.179704085087488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00509039341953732</t>
+    <t xml:space="preserve">-0.179704085087489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00509039341953729</t>
   </si>
   <si>
     <t xml:space="preserve">0.163178512971034</t>
@@ -779,70 +779,70 @@
     <t xml:space="preserve">-0.198262037085476</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00491842190486535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000731309249960727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0329744612013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.160249236587387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.149308601524815</t>
+    <t xml:space="preserve">-0.00491842190486531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000731309249960996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0329744612013005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.160249236587388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.149308601524814</t>
   </si>
   <si>
     <t xml:space="preserve">0.344110088291943</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.220403638680766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.245257253086964</t>
+    <t xml:space="preserve">-0.220403638680767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.245257253086963</t>
   </si>
   <si>
     <t xml:space="preserve">0.392434381092845</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.412709691796924</t>
+    <t xml:space="preserve">-0.412709691796925</t>
   </si>
   <si>
     <t xml:space="preserve">-0.462008458850862</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0230060251622761</t>
+    <t xml:space="preserve">0.0230060251622762</t>
   </si>
   <si>
     <t xml:space="preserve">-0.51147292231191</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0832266634578486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0752816554266597</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.486255622515939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.00756706921689201</t>
+    <t xml:space="preserve">-0.0832266634578485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0752816554266599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.486255622515938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.00756706921689213</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0345633827476928</t>
   </si>
   <si>
-    <t xml:space="preserve">0.050760390013205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.021413473890779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0434710467042603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0669787452046164</t>
+    <t xml:space="preserve">0.0507603900132044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0214134738907788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0434710467042601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0669787452046161</t>
   </si>
   <si>
     <t xml:space="preserve">0.110608018109106</t>
@@ -854,52 +854,52 @@
     <t xml:space="preserve">0.437499797647647</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0699560996757538</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.418302850041387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0404059464523273</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0570369274761526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0984496033339913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.103164898693531</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.069814091452431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0583761796600291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0355116724479259</t>
+    <t xml:space="preserve">-0.0699560996757531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.418302850041388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0404059464523267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0570369274761525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0984496033339909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.103164898693532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0698140914524312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0583761796600293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0355116724479262</t>
   </si>
   <si>
     <t xml:space="preserve">-0.185932499213256</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.00768682686829945</t>
+    <t xml:space="preserve">-0.0076868268682995</t>
   </si>
   <si>
     <t xml:space="preserve">-0.107114224104493</t>
   </si>
   <si>
-    <t xml:space="preserve">0.390099666605516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0038467088578318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0305854991483806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.112554463430331</t>
+    <t xml:space="preserve">0.390099666605517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00384670885783176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0305854991483807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.112554463430332</t>
   </si>
   <si>
     <t xml:space="preserve">-0.581458877831682</t>
@@ -911,7 +911,7 @@
     <t xml:space="preserve">0.114974881097731</t>
   </si>
   <si>
-    <t xml:space="preserve">0.588469879064147</t>
+    <t xml:space="preserve">0.588469879064148</t>
   </si>
   <si>
     <t xml:space="preserve">-0.15169366629802</t>
@@ -920,34 +920,34 @@
     <t xml:space="preserve">-0.0223622870674415</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.147578230248496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0392686629911767</t>
+    <t xml:space="preserve">-0.147578230248495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0392686629911759</t>
   </si>
   <si>
     <t xml:space="preserve">0.0710121693113409</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0298391954715029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0195353861806116</t>
+    <t xml:space="preserve">0.029839195471503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0195353861806118</t>
   </si>
   <si>
     <t xml:space="preserve">-0.317426995320424</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0708195379107086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00410891219953283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0790083777227833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.191289963235943</t>
+    <t xml:space="preserve">0.0708195379107083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00410891219953281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0790083777227831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.191289963235942</t>
   </si>
   <si>
     <t xml:space="preserve">0.0178080606452021</t>
@@ -956,10 +956,10 @@
     <t xml:space="preserve">0.0241912268063363</t>
   </si>
   <si>
-    <t xml:space="preserve">0.01747300191601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0228690293729326</t>
+    <t xml:space="preserve">0.0174730019160098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0228690293729319</t>
   </si>
   <si>
     <t xml:space="preserve">-0.109715054651705</t>
@@ -968,13 +968,13 @@
     <t xml:space="preserve">0.247358949578326</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0501652110699539</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.208978135613687</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.056103852869937</t>
+    <t xml:space="preserve">-0.050165211069953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.208978135613688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0561038528699371</t>
   </si>
   <si>
     <t xml:space="preserve">-0.532702659866491</t>
@@ -983,13 +983,13 @@
     <t xml:space="preserve">0.663992390535628</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0339569657661885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.3306627445559</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0763858986304453</t>
+    <t xml:space="preserve">0.0339569657661886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.330662744555899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0763858986304451</t>
   </si>
   <si>
     <t xml:space="preserve">-0.11048863269772</t>
@@ -998,22 +998,22 @@
     <t xml:space="preserve">0.568497364664159</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00398377208043598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0392141968089541</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.338642707363422</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0210348455172964</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0407705870531167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0237683547185793</t>
+    <t xml:space="preserve">0.00398377208043602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0392141968089539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.338642707363421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0210348455172962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0407705870531164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0237683547185796</t>
   </si>
   <si>
     <t xml:space="preserve">-0.408263864900699</t>
@@ -1022,28 +1022,28 @@
     <t xml:space="preserve">-0.158443908946349</t>
   </si>
   <si>
-    <t xml:space="preserve">0.254042460774401</t>
+    <t xml:space="preserve">0.2540424607744</t>
   </si>
   <si>
     <t xml:space="preserve">0.105977135871593</t>
   </si>
   <si>
-    <t xml:space="preserve">0.270245085446128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.168473390756012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.053747614340936</t>
+    <t xml:space="preserve">0.270245085446127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.168473390756013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0537476143409355</t>
   </si>
   <si>
     <t xml:space="preserve">-0.179708641298495</t>
   </si>
   <si>
-    <t xml:space="preserve">0.162406689795235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0665150644556139</t>
+    <t xml:space="preserve">0.162406689795236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0665150644556144</t>
   </si>
   <si>
     <t xml:space="preserve">-0.0207529958212271</t>
@@ -1052,40 +1052,40 @@
     <t xml:space="preserve">0.109578914595145</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.0744068446517152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0084766866505837</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.000783306696191055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0455418912541566</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.000878509257946247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0173887767821313</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.013958189439793</t>
+    <t xml:space="preserve">-0.0744068446517149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00847668665058336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.000783306696191217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0455418912541574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.000878509257945998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0173887767821311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0139581894397936</t>
   </si>
   <si>
     <t xml:space="preserve">0.221806585012749</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0190552720971748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0611856151811289</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.01396214586827</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.0888470334794377</t>
+    <t xml:space="preserve">0.0190552720971743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0611856151811291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0139621458682704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0888470334794383</t>
   </si>
   <si>
     <t xml:space="preserve">-0.470887229281481</t>
@@ -1097,7 +1097,7 @@
     <t xml:space="preserve">-0.177731042380354</t>
   </si>
   <si>
-    <t xml:space="preserve">0.789008763143682</t>
+    <t xml:space="preserve">0.789008763143683</t>
   </si>
 </sst>
 </file>

</xml_diff>